<commit_message>
Mock  dados quando não consegue entrar na api
</commit_message>
<xml_diff>
--- a/Requisitos funcionais - Pizzaria .xlsx
+++ b/Requisitos funcionais - Pizzaria .xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28015"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28223"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Guilherme\Desktop\Pizzaria\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DCAB0A4-D694-4C7D-9B3D-AD8FE437F057}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E625422-D516-4447-90BF-02A01939F363}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="3825" yWindow="1845" windowWidth="21600" windowHeight="11385" xr2:uid="{EEB73612-4382-4C6F-89B4-D44344F8DD0B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="602" xr2:uid="{EEB73612-4382-4C6F-89B4-D44344F8DD0B}"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="V1" sheetId="1" r:id="rId1"/>
+    <sheet name="V1.1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="74">
   <si>
     <t>ID</t>
   </si>
@@ -216,13 +217,55 @@
   </si>
   <si>
     <t>Alterar informações de um cliente especifico</t>
+  </si>
+  <si>
+    <t>Cadastrar pedido</t>
+  </si>
+  <si>
+    <t>Cadastrar pedido no sistema</t>
+  </si>
+  <si>
+    <t>ALTA</t>
+  </si>
+  <si>
+    <t>Consultar pedido</t>
+  </si>
+  <si>
+    <t>Consultar a lista de pedidos</t>
+  </si>
+  <si>
+    <t>Cancelar pedido</t>
+  </si>
+  <si>
+    <t>Cancelar um pedido em andamento</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carregar pizzas </t>
+  </si>
+  <si>
+    <t>Carregar pizzas para novo pedido</t>
+  </si>
+  <si>
+    <t>Carregar ultimos pedidos</t>
+  </si>
+  <si>
+    <t>Carregar os ultimos pedidos feitos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RF6 </t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>Entrar com as credenciais</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -245,6 +288,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -313,7 +364,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center"/>
@@ -327,6 +378,9 @@
     <xf numFmtId="14" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
@@ -668,10 +722,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{724EE660-9F26-49CF-8530-09FB5138432D}">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -690,42 +744,42 @@
       <c r="A1" s="1"/>
     </row>
     <row r="2" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="8" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-    </row>
-    <row r="4" spans="1:8" ht="52.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="9"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+    </row>
+    <row r="4" spans="1:8" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
@@ -751,7 +805,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>14</v>
       </c>
@@ -799,7 +853,9 @@
       <c r="G6" s="4">
         <v>45521</v>
       </c>
-      <c r="H6" s="2"/>
+      <c r="H6" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="7" spans="1:8" ht="36.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
@@ -823,7 +879,9 @@
       <c r="G7" s="4">
         <v>45521</v>
       </c>
-      <c r="H7" s="2"/>
+      <c r="H7" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="8" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
@@ -847,7 +905,9 @@
       <c r="G8" s="4">
         <v>45521</v>
       </c>
-      <c r="H8" s="2"/>
+      <c r="H8" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="9" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
@@ -871,7 +931,9 @@
       <c r="G9" s="4">
         <v>45521</v>
       </c>
-      <c r="H9" s="2"/>
+      <c r="H9" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="10" spans="1:8" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
@@ -895,7 +957,9 @@
       <c r="G10" s="4">
         <v>45521</v>
       </c>
-      <c r="H10" s="2"/>
+      <c r="H10" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="11" spans="1:8" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
@@ -919,7 +983,9 @@
       <c r="G11" s="4">
         <v>45521</v>
       </c>
-      <c r="H11" s="2"/>
+      <c r="H11" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="12" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
@@ -943,7 +1009,9 @@
       <c r="G12" s="4">
         <v>45521</v>
       </c>
-      <c r="H12" s="2"/>
+      <c r="H12" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="13" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
@@ -967,7 +1035,9 @@
       <c r="G13" s="4">
         <v>45521</v>
       </c>
-      <c r="H13" s="2"/>
+      <c r="H13" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="14" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
@@ -991,7 +1061,9 @@
       <c r="G14" s="4">
         <v>45521</v>
       </c>
-      <c r="H14" s="2"/>
+      <c r="H14" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="15" spans="1:8" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
@@ -1015,7 +1087,9 @@
       <c r="G15" s="4">
         <v>45521</v>
       </c>
-      <c r="H15" s="2"/>
+      <c r="H15" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="16" spans="1:8" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
@@ -1091,7 +1165,9 @@
       <c r="G18" s="4">
         <v>45521</v>
       </c>
-      <c r="H18" s="2"/>
+      <c r="H18" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="19" spans="1:8" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
@@ -1115,7 +1191,9 @@
       <c r="G19" s="4">
         <v>45521</v>
       </c>
-      <c r="H19" s="2"/>
+      <c r="H19" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="20" spans="1:8" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
@@ -1139,7 +1217,9 @@
       <c r="G20" s="4">
         <v>45521</v>
       </c>
-      <c r="H20" s="2"/>
+      <c r="H20" s="2" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="21" spans="1:8" ht="42" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
@@ -1163,7 +1243,14 @@
       <c r="G21" s="4">
         <v>45521</v>
       </c>
-      <c r="H21" s="2"/>
+      <c r="H21" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -1180,4 +1267,187 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0360D92E-8349-4346-850A-36E4398D2262}">
+  <dimension ref="A1:H8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" s="5">
+        <v>45591</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E4" s="5">
+        <v>45591</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="6"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D5" t="s">
+        <v>62</v>
+      </c>
+      <c r="E5" s="5">
+        <v>45591</v>
+      </c>
+      <c r="F5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E6" s="5">
+        <v>45591</v>
+      </c>
+      <c r="F6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" t="s">
+        <v>70</v>
+      </c>
+      <c r="D7" t="s">
+        <v>62</v>
+      </c>
+      <c r="E7" s="5">
+        <v>45591</v>
+      </c>
+      <c r="F7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C8" t="s">
+        <v>73</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="E8" s="5">
+        <v>45591</v>
+      </c>
+      <c r="F8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="E1:E2"/>
+    <mergeCell ref="F1:F2"/>
+  </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>